<commit_message>
w mainie napisane co zrobic
</commit_message>
<xml_diff>
--- a/Files/insertionSort.xlsx
+++ b/Files/insertionSort.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1_studia\AiZO\Projekt1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1_studia\AiZO\Projekt1\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3E3D24-F5A5-4517-A17E-2FAB454DC57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D53954-8B3B-42E1-8920-50D92C97A0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EF58670-48A2-47F8-B1A0-2E5F79361CDD}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -136,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -486,47 +492,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1958,16 +1960,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1104900</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>22412</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>193862</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:rowOff>145116</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2314,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D357065D-6118-472C-A97E-77F1867B67D4}">
   <dimension ref="A2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2326,7 @@
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2479,339 +2481,339 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="A24" s="4">
         <v>10000</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="5">
         <v>151.6</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
+      <c r="A25" s="6">
         <v>20000</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="7">
         <v>660.2</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="A26" s="4">
         <v>40000</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="5">
         <v>2922.8</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+      <c r="A27" s="6">
         <v>80000</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="7">
         <v>10636.4</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11">
+      <c r="A28" s="4">
         <v>160000</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="5">
         <v>46217.8</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="6">
         <v>320000</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="7">
         <v>187300</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="31" cm="1">
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="14" cm="1">
         <f t="array" ref="H29:N30">TRANSPOSE(A4:B10)</f>
         <v>10000</v>
       </c>
-      <c r="I29" s="32">
+      <c r="I29" s="15">
         <v>20000</v>
       </c>
-      <c r="J29" s="32">
+      <c r="J29" s="15">
         <v>40000</v>
       </c>
-      <c r="K29" s="32">
+      <c r="K29" s="15">
         <v>80000</v>
       </c>
-      <c r="L29" s="32">
+      <c r="L29" s="15">
         <v>160000</v>
       </c>
-      <c r="M29" s="32">
+      <c r="M29" s="15">
         <v>320000</v>
       </c>
-      <c r="N29" s="33">
+      <c r="N29" s="16">
         <v>640000</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="A30" s="4">
         <v>640000</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="5">
         <v>928634</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="29" t="s">
+      <c r="F30" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="18" t="s">
+      <c r="G30" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="28">
+      <c r="H30" s="23">
         <v>77.92</v>
       </c>
-      <c r="I30" s="29">
+      <c r="I30" s="21">
         <v>347.46</v>
       </c>
-      <c r="J30" s="29">
+      <c r="J30" s="21">
         <v>1438.72</v>
       </c>
-      <c r="K30" s="29">
+      <c r="K30" s="21">
         <v>5799.86</v>
       </c>
-      <c r="L30" s="29">
+      <c r="L30" s="21">
         <v>24715.1</v>
       </c>
-      <c r="M30" s="29">
+      <c r="M30" s="21">
         <v>104136</v>
       </c>
-      <c r="N30" s="30">
+      <c r="N30" s="24">
         <v>481520</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="16">
+      <c r="A31" s="12">
         <v>0.33</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="22" t="s">
+      <c r="B31" s="5"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="23" cm="1">
+      <c r="G31" s="22"/>
+      <c r="H31" s="26" cm="1">
         <f t="array" ref="H31:N31">TRANSPOSE(B14:B20)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I31" s="25">
         <v>0</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J31" s="25">
         <v>0</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K31" s="25">
         <v>0</v>
       </c>
-      <c r="L31" s="22">
+      <c r="L31" s="25">
         <v>0</v>
       </c>
-      <c r="M31" s="22">
+      <c r="M31" s="25">
         <v>1</v>
       </c>
-      <c r="N31" s="24">
+      <c r="N31" s="27">
         <v>1.4</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
+      <c r="A32" s="6">
         <v>10000</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="7">
         <v>70.400000000000006</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="22" t="s">
+      <c r="E32" s="20"/>
+      <c r="F32" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="23" cm="1">
+      <c r="G32" s="22"/>
+      <c r="H32" s="26" cm="1">
         <f t="array" ref="H32:N32">TRANSPOSE(B24:B30)</f>
         <v>151.6</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I32" s="25">
         <v>660.2</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J32" s="25">
         <v>2922.8</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K32" s="25">
         <v>10636.4</v>
       </c>
-      <c r="L32" s="22">
+      <c r="L32" s="25">
         <v>46217.8</v>
       </c>
-      <c r="M32" s="22">
+      <c r="M32" s="25">
         <v>187300</v>
       </c>
-      <c r="N32" s="24">
+      <c r="N32" s="27">
         <v>928634</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
+      <c r="A33" s="4">
         <v>20000</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="5">
         <v>277.8</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="22" t="s">
+      <c r="E33" s="20"/>
+      <c r="F33" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="18"/>
-      <c r="H33" s="23" cm="1">
+      <c r="G33" s="22"/>
+      <c r="H33" s="26" cm="1">
         <f t="array" ref="H33:N33">TRANSPOSE(B32:B38)</f>
         <v>70.400000000000006</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I33" s="25">
         <v>277.8</v>
       </c>
-      <c r="J33" s="22">
+      <c r="J33" s="25">
         <v>1122.5999999999999</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K33" s="25">
         <v>4609</v>
       </c>
-      <c r="L33" s="22">
+      <c r="L33" s="25">
         <v>22263</v>
       </c>
-      <c r="M33" s="22">
+      <c r="M33" s="25">
         <v>96701.2</v>
       </c>
-      <c r="N33" s="24">
+      <c r="N33" s="27">
         <v>400550</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13">
+      <c r="A34" s="6">
         <v>40000</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="7">
         <v>1122.5999999999999</v>
       </c>
-      <c r="E34" s="35"/>
-      <c r="F34" s="26" t="s">
+      <c r="E34" s="28"/>
+      <c r="F34" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="25" cm="1">
+      <c r="G34" s="30"/>
+      <c r="H34" s="31" cm="1">
         <f t="array" ref="H34:N34">TRANSPOSE(B40:B46)</f>
         <v>45.8</v>
       </c>
-      <c r="I34" s="26">
+      <c r="I34" s="29">
         <v>187.4</v>
       </c>
-      <c r="J34" s="26">
+      <c r="J34" s="29">
         <v>680.2</v>
       </c>
-      <c r="K34" s="26">
+      <c r="K34" s="29">
         <v>3135.6</v>
       </c>
-      <c r="L34" s="26">
+      <c r="L34" s="29">
         <v>11930.8</v>
       </c>
-      <c r="M34" s="26">
+      <c r="M34" s="29">
         <v>58201.599999999999</v>
       </c>
-      <c r="N34" s="27">
+      <c r="N34" s="32">
         <v>252226</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
+      <c r="A35" s="4">
         <v>80000</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="5">
         <v>4609</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
+      <c r="A36" s="6">
         <v>160000</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="7">
         <v>22263</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+      <c r="A37" s="4">
         <v>320000</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="5">
         <v>96701.2</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="13">
+      <c r="A38" s="6">
         <v>640000</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="7">
         <v>400550</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
+      <c r="A39" s="13">
         <v>0.66</v>
       </c>
-      <c r="B39" s="14"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
+      <c r="A40" s="4">
         <v>10000</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="5">
         <v>45.8</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="13">
+      <c r="A41" s="6">
         <v>20000</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="7">
         <v>187.4</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="11">
+      <c r="A42" s="4">
         <v>40000</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="5">
         <v>680.2</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="13">
+      <c r="A43" s="6">
         <v>80000</v>
       </c>
-      <c r="B43" s="14">
+      <c r="B43" s="7">
         <v>3135.6</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
+      <c r="A44" s="4">
         <v>160000</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="5">
         <v>11930.8</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="13">
+      <c r="A45" s="6">
         <v>320000</v>
       </c>
-      <c r="B45" s="14">
+      <c r="B45" s="7">
         <v>58201.599999999999</v>
       </c>
     </row>
@@ -2819,7 +2821,7 @@
       <c r="A46" s="10">
         <v>640000</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="11">
         <v>252226</v>
       </c>
     </row>

</xml_diff>